<commit_message>
final commit minus testing and misc updates
</commit_message>
<xml_diff>
--- a/data/calcs/relief_calcs/season_mu_std.xlsx
+++ b/data/calcs/relief_calcs/season_mu_std.xlsx
@@ -477,25 +477,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.856595744680852</v>
+        <v>5.463630573248407</v>
       </c>
       <c r="C2" t="n">
-        <v>1.390973883572568</v>
+        <v>2.240568743774976</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9647241327751196</v>
+        <v>1.322903771964442</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4773101076555024</v>
+        <v>0.7159837955602021</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5428939892344498</v>
+        <v>0.6407549044741776</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.4822692384370016</v>
+        <v>-0.4845913390137646</v>
       </c>
       <c r="H2" t="n">
-        <v>25.5</v>
+        <v>25.35414012738854</v>
       </c>
     </row>
     <row r="3">
@@ -505,25 +505,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.012668185914867</v>
+        <v>4.633661436405054</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7710224487531796</v>
+        <v>1.683809642222656</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3964093900324763</v>
+        <v>0.8144442427531886</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1321134012105241</v>
+        <v>0.5966637052870977</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1511331064038821</v>
+        <v>0.5497627707135105</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2023152211916691</v>
+        <v>0.8797663191006361</v>
       </c>
       <c r="H3" t="n">
-        <v>19.14605516996722</v>
+        <v>25.17899060047703</v>
       </c>
     </row>
     <row r="4">
@@ -533,25 +533,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.251509433962264</v>
+        <v>5.231111111111111</v>
       </c>
       <c r="C4" t="n">
-        <v>1.833867010766729</v>
+        <v>2.311781089734088</v>
       </c>
       <c r="D4" t="n">
-        <v>1.365235215333583</v>
+        <v>1.295143358830755</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9275340821386783</v>
+        <v>0.7691535895238956</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6017599952851432</v>
+        <v>0.5403056057900927</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.4484816159809507</v>
+        <v>-0.4549955092976475</v>
       </c>
       <c r="H4" t="n">
-        <v>35.125</v>
+        <v>24.35636856368564</v>
       </c>
     </row>
     <row r="5">
@@ -561,25 +561,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.211633348047831</v>
+        <v>4.720194510067887</v>
       </c>
       <c r="C5" t="n">
-        <v>1.685498202578049</v>
+        <v>1.7711033548038</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5570616445305397</v>
+        <v>0.8911236331312969</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6100793432578291</v>
+        <v>0.6063470312657683</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3165990979509523</v>
+        <v>0.4324091930454509</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6372786881767656</v>
+        <v>0.8113933948058411</v>
       </c>
       <c r="H5" t="n">
-        <v>33.5790644811402</v>
+        <v>24.21593482427432</v>
       </c>
     </row>
     <row r="6">
@@ -589,25 +589,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.197692307692307</v>
+        <v>5.521489932885906</v>
       </c>
       <c r="C6" t="n">
-        <v>1.979397761301615</v>
+        <v>2.443767023738328</v>
       </c>
       <c r="D6" t="n">
-        <v>1.125522514366197</v>
+        <v>1.350303711758079</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5956844908491161</v>
+        <v>0.7956553141680518</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5292202421171368</v>
+        <v>0.6276022584510498</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.5590969144459537</v>
+        <v>-0.5169876928642829</v>
       </c>
       <c r="H6" t="n">
-        <v>36.125</v>
+        <v>25.55704697986577</v>
       </c>
     </row>
     <row r="7">
@@ -617,25 +617,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.781673167564158</v>
+        <v>4.749391535190125</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9404541246601121</v>
+        <v>1.789747079028432</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3474999627343497</v>
+        <v>0.829383928103861</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1251872369958739</v>
+        <v>0.5885783525344821</v>
       </c>
       <c r="F7" t="n">
-        <v>0.240828974686066</v>
+        <v>0.5083603725834306</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2689092288023822</v>
+        <v>0.815415571167421</v>
       </c>
       <c r="H7" t="n">
-        <v>26.36793236381755</v>
+        <v>25.18164722291512</v>
       </c>
     </row>
     <row r="8">
@@ -645,25 +645,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.884923076923076</v>
+        <v>5.100556492411467</v>
       </c>
       <c r="C8" t="n">
-        <v>2.005764577520506</v>
+        <v>2.258784850519582</v>
       </c>
       <c r="D8" t="n">
-        <v>1.059037370656025</v>
+        <v>1.275894941232602</v>
       </c>
       <c r="E8" t="n">
-        <v>0.542980925246811</v>
+        <v>0.7613507843784619</v>
       </c>
       <c r="F8" t="n">
-        <v>0.355634708221188</v>
+        <v>0.5336702779734646</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.714069491952032</v>
+        <v>-0.4173430637859449</v>
       </c>
       <c r="H8" t="n">
-        <v>49.57142857142857</v>
+        <v>29.81281618887015</v>
       </c>
     </row>
     <row r="9">
@@ -673,25 +673,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.54828647530597</v>
+        <v>4.484853849112721</v>
       </c>
       <c r="C9" t="n">
-        <v>1.46430843738422</v>
+        <v>1.697809794214145</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2721539148269986</v>
+        <v>0.8562049726558092</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2414876386139475</v>
+        <v>0.5345199867736541</v>
       </c>
       <c r="F9" t="n">
-        <v>0.09680185225817421</v>
+        <v>0.4178948825234093</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6116258030479832</v>
+        <v>0.6975964498132601</v>
       </c>
       <c r="H9" t="n">
-        <v>31.16545706845504</v>
+        <v>26.98104385230003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>